<commit_message>
setting up for fall testing
</commit_message>
<xml_diff>
--- a/Kid Choice Experiments/Remaining Kids Checklist.xlsx
+++ b/Kid Choice Experiments/Remaining Kids Checklist.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="54">
   <si>
     <t>&gt; with(Parent34, tapply(as.numeric(as.character(Include.subject.)), list(Condition, Age.Years, Gender), sum.na.rm), drop=TRUE)</t>
   </si>
@@ -136,6 +137,51 @@
   </si>
   <si>
     <t>6M</t>
+  </si>
+  <si>
+    <t>ParentSecret:</t>
+  </si>
+  <si>
+    <t>6 SDOD 6yos</t>
+  </si>
+  <si>
+    <t>2 ODSD 3yos</t>
+  </si>
+  <si>
+    <t>6 ODSD 3yos</t>
+  </si>
+  <si>
+    <t>3 ODSD 4yos</t>
+  </si>
+  <si>
+    <t>3 SDOD 4yos</t>
+  </si>
+  <si>
+    <t>ParentSecretControl:</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Age/Gender</t>
+  </si>
+  <si>
+    <t>ParentSecret</t>
+  </si>
+  <si>
+    <t>SDOD</t>
+  </si>
+  <si>
+    <t>ODSD</t>
+  </si>
+  <si>
+    <t>ParentSecretControl</t>
+  </si>
+  <si>
+    <t>4M</t>
+  </si>
+  <si>
+    <t>4F</t>
   </si>
 </sst>
 </file>
@@ -181,7 +227,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -324,15 +370,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -343,12 +493,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -680,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1296,4 +1472,307 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28" customHeight="1" thickBot="1">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28" customHeight="1">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" ht="28" customHeight="1">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" ht="28" customHeight="1">
+      <c r="C4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" ht="28" customHeight="1">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" ht="28" customHeight="1">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" ht="28" customHeight="1">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" ht="28" customHeight="1">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" ht="28" customHeight="1">
+      <c r="C9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" ht="28" customHeight="1">
+      <c r="C10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" ht="28" customHeight="1">
+      <c r="C11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" ht="28" customHeight="1">
+      <c r="C12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" ht="28" customHeight="1">
+      <c r="C13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" ht="28" customHeight="1">
+      <c r="C14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" ht="28" customHeight="1">
+      <c r="C15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" ht="28" customHeight="1">
+      <c r="C16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="3:6" ht="28" customHeight="1">
+      <c r="C17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="3:6" ht="28" customHeight="1">
+      <c r="C18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="3:6" ht="28" customHeight="1">
+      <c r="C19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="3:6" ht="28" customHeight="1">
+      <c r="C20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="3:6" ht="28" customHeight="1" thickBot="1">
+      <c r="C21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="9"/>
+    </row>
+  </sheetData>
+  <sortState ref="C2:F21">
+    <sortCondition ref="C2:C21"/>
+  </sortState>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>